<commit_message>
excel corrections and add cedula
</commit_message>
<xml_diff>
--- a/Ejemplo_importar_usuarios.xlsx
+++ b/Ejemplo_importar_usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juano\Documents\Proyectos\Prueba\sgvp_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juano\Documents\Proyectos\sgvp_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660967CF-BE89-4179-B4BD-BFA132C2E936}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DD1F44-380B-4D28-9F5B-300824250237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{51DC1C1F-A0F5-4F43-B435-E1A455174F4C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>juan</t>
   </si>
@@ -66,13 +66,16 @@
   </si>
   <si>
     <t>estudiante2@hotmail.com</t>
+  </si>
+  <si>
+    <t>cedula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +87,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,9 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -428,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733ABEC5-A2BB-4C74-B092-C163920B27B8}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G5" sqref="G5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -449,8 +461,11 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -463,8 +478,11 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E2">
+        <v>123123123</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -477,6 +495,12 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E3">
+        <v>12312313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -484,5 +508,6 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{A66E8FB3-E146-471B-9A86-A3F2BCBC49E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>